<commit_message>
commit de teste para slack
</commit_message>
<xml_diff>
--- a/Relatorio_Lab2/Testes de processadores.xlsx
+++ b/Relatorio_Lab2/Testes de processadores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nmac\Documents\GitHub\AAC-e-ERap\Relatorio_Lab2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margarida\Downloads\git\AAC-e-ERap\Relatorio_Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -193,7 +193,7 @@
     <t>Teste #3</t>
   </si>
   <si>
-    <t>Processador #5</t>
+    <t>Processador Demonstrado</t>
   </si>
 </sst>
 </file>
@@ -252,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +271,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -422,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -460,6 +466,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,43 +527,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +548,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -803,28 +812,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AB27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D19" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" customWidth="1"/>
+    <col min="6" max="6" width="4.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" customWidth="1"/>
+    <col min="9" max="9" width="19.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:28" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="34" t="s">
+    <row r="2" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="2:28" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
@@ -834,14 +843,14 @@
       <c r="I3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="N3" s="29" t="s">
+      <c r="K3" s="25"/>
+      <c r="N3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="29"/>
+      <c r="O3" s="28"/>
       <c r="P3" s="2" t="s">
         <v>4</v>
       </c>
@@ -851,15 +860,15 @@
       <c r="R3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="29" t="s">
+      <c r="S3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="29"/>
+      <c r="T3" s="28"/>
       <c r="U3" s="3"/>
-      <c r="V3" s="29" t="s">
+      <c r="V3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="29"/>
+      <c r="W3" s="28"/>
       <c r="X3" s="2" t="s">
         <v>4</v>
       </c>
@@ -869,16 +878,16 @@
       <c r="Z3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA3" s="29" t="s">
+      <c r="AA3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="29"/>
-    </row>
-    <row r="4" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="35" t="s">
+      <c r="AB3" s="28"/>
+    </row>
+    <row r="4" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="15">
         <v>211.33799999999999</v>
       </c>
@@ -888,15 +897,15 @@
       <c r="I4" s="15">
         <v>0</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="19">
         <f>(1/(G4))*H4</f>
         <v>0.26971013258382309</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="N4" s="29" t="s">
+      <c r="K4" s="19"/>
+      <c r="N4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="29"/>
+      <c r="O4" s="28"/>
       <c r="P4" s="1">
         <v>211.33799999999999</v>
       </c>
@@ -906,16 +915,16 @@
       <c r="R4" s="1">
         <v>108</v>
       </c>
-      <c r="S4" s="30">
+      <c r="S4" s="29">
         <f>(1/(P4))*Q4</f>
         <v>11.157482326888681</v>
       </c>
-      <c r="T4" s="30"/>
+      <c r="T4" s="29"/>
       <c r="U4" s="3"/>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="29"/>
+      <c r="W4" s="28"/>
       <c r="X4" s="1">
         <v>211.33799999999999</v>
       </c>
@@ -925,17 +934,17 @@
       <c r="Z4" s="1">
         <v>122</v>
       </c>
-      <c r="AA4" s="30">
+      <c r="AA4" s="29">
         <f>(1/(X4))*Y4</f>
         <v>5.0061986012927164</v>
       </c>
-      <c r="AB4" s="30"/>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="35" t="s">
+      <c r="AB4" s="29"/>
+    </row>
+    <row r="5" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="15">
         <v>211.33799999999999</v>
       </c>
@@ -945,15 +954,15 @@
       <c r="I5" s="15">
         <v>0</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="19">
         <f t="shared" ref="J5:J7" si="0">(1/(G5))*H5</f>
         <v>0.53942026516764618</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="N5" s="29" t="s">
+      <c r="K5" s="19"/>
+      <c r="N5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="29"/>
+      <c r="O5" s="28"/>
       <c r="P5" s="1">
         <v>211.33799999999999</v>
       </c>
@@ -963,16 +972,16 @@
       <c r="R5" s="1">
         <v>108</v>
       </c>
-      <c r="S5" s="30">
+      <c r="S5" s="29">
         <f t="shared" ref="S5:S7" si="1">(1/(P5))*Q5</f>
         <v>14.403467431318553</v>
       </c>
-      <c r="T5" s="30"/>
+      <c r="T5" s="29"/>
       <c r="U5" s="3"/>
-      <c r="V5" s="29" t="s">
+      <c r="V5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="W5" s="29"/>
+      <c r="W5" s="28"/>
       <c r="X5" s="1">
         <v>211.33799999999999</v>
       </c>
@@ -982,17 +991,17 @@
       <c r="Z5" s="1">
         <v>122</v>
       </c>
-      <c r="AA5" s="30">
+      <c r="AA5" s="29">
         <f t="shared" ref="AA5:AA7" si="2">(1/(X5))*Y5</f>
         <v>7.4856391183790905</v>
       </c>
-      <c r="AB5" s="30"/>
-    </row>
-    <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="35" t="s">
+      <c r="AB5" s="29"/>
+    </row>
+    <row r="6" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="15">
         <v>285.608</v>
       </c>
@@ -1002,15 +1011,15 @@
       <c r="I6" s="15">
         <v>0</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="19">
         <f t="shared" si="0"/>
         <v>0.19957424161788187</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="N6" s="29" t="s">
+      <c r="K6" s="19"/>
+      <c r="N6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="29"/>
+      <c r="O6" s="28"/>
       <c r="P6" s="4">
         <v>285.608</v>
       </c>
@@ -1020,16 +1029,16 @@
       <c r="R6" s="1">
         <v>463</v>
       </c>
-      <c r="S6" s="30">
+      <c r="S6" s="29">
         <f t="shared" si="1"/>
         <v>9.4710232206380773</v>
       </c>
-      <c r="T6" s="30"/>
+      <c r="T6" s="29"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="29" t="s">
+      <c r="V6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="W6" s="29"/>
+      <c r="W6" s="28"/>
       <c r="X6" s="4">
         <v>285.608</v>
       </c>
@@ -1039,17 +1048,17 @@
       <c r="Z6" s="1">
         <v>187</v>
       </c>
-      <c r="AA6" s="30">
+      <c r="AA6" s="29">
         <f t="shared" si="2"/>
         <v>3.931962690120725</v>
       </c>
-      <c r="AB6" s="30"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="36" t="s">
+      <c r="AB6" s="29"/>
+    </row>
+    <row r="7" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="16">
         <v>285.608</v>
       </c>
@@ -1059,15 +1068,15 @@
       <c r="I7" s="16">
         <v>0</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="27">
         <f t="shared" si="0"/>
         <v>0.39914848323576374</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="N7" s="29" t="s">
+      <c r="K7" s="27"/>
+      <c r="N7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="29"/>
+      <c r="O7" s="28"/>
       <c r="P7" s="4">
         <v>285.608</v>
       </c>
@@ -1077,16 +1086,16 @@
       <c r="R7" s="1">
         <v>463</v>
       </c>
-      <c r="S7" s="30">
+      <c r="S7" s="29">
         <f t="shared" si="1"/>
         <v>11.634828156074061</v>
       </c>
-      <c r="T7" s="30"/>
+      <c r="T7" s="29"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="29" t="s">
+      <c r="V7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="W7" s="29"/>
+      <c r="W7" s="28"/>
       <c r="X7" s="4">
         <v>285.608</v>
       </c>
@@ -1096,18 +1105,18 @@
       <c r="Z7" s="1">
         <v>187</v>
       </c>
-      <c r="AA7" s="30">
+      <c r="AA7" s="29">
         <f t="shared" si="2"/>
         <v>5.7666451920114286</v>
       </c>
-      <c r="AB7" s="30"/>
-    </row>
-    <row r="8" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:28" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="25" t="s">
+      <c r="AB7" s="29"/>
+    </row>
+    <row r="8" spans="2:28" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="2:28" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1117,16 +1126,16 @@
       <c r="I9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="17" t="s">
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="15">
         <v>211.33799999999999</v>
       </c>
@@ -1136,23 +1145,23 @@
       <c r="I10" s="15">
         <v>108</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="32">
         <f>(1/(G10))*H10</f>
         <v>11.157482326888681</v>
       </c>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="33"/>
+    </row>
+    <row r="11" spans="2:28" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="15">
         <v>211.33799999999999</v>
       </c>
@@ -1162,23 +1171,23 @@
       <c r="I11" s="15">
         <v>108</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="32">
         <f t="shared" ref="J11:J13" si="3">(1/(G11))*H11</f>
         <v>14.403467431318553</v>
       </c>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="33"/>
+    </row>
+    <row r="12" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="15">
         <v>285.608</v>
       </c>
@@ -1188,23 +1197,23 @@
       <c r="I12" s="15">
         <v>463</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="32">
         <f t="shared" si="3"/>
         <v>9.4710232206380773</v>
       </c>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="33"/>
+    </row>
+    <row r="13" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="16">
         <v>285.608</v>
       </c>
@@ -1214,13 +1223,13 @@
       <c r="I13" s="16">
         <v>463</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="36">
         <f t="shared" si="3"/>
         <v>11.634828156074061</v>
       </c>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="37"/>
+    </row>
+    <row r="14" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
@@ -1228,11 +1237,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:28" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="25" t="s">
+    <row r="15" spans="2:28" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="11" t="s">
         <v>10</v>
       </c>
@@ -1242,16 +1251,16 @@
       <c r="I15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="28"/>
-    </row>
-    <row r="16" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="17" t="s">
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E16" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="15">
         <v>211.33799999999999</v>
       </c>
@@ -1261,17 +1270,17 @@
       <c r="I16" s="15">
         <v>122</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="32">
         <f>(1/(G16))*H16</f>
         <v>5.0061986012927164</v>
       </c>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="17" t="s">
+      <c r="K16" s="33"/>
+    </row>
+    <row r="17" spans="5:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E17" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="15">
         <v>211.33799999999999</v>
       </c>
@@ -1281,17 +1290,17 @@
       <c r="I17" s="15">
         <v>122</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="32">
         <f t="shared" ref="J17:J19" si="4">(1/(G17))*H17</f>
         <v>7.4856391183790905</v>
       </c>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="17" t="s">
+      <c r="K17" s="33"/>
+    </row>
+    <row r="18" spans="5:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="15">
         <v>285.608</v>
       </c>
@@ -1301,17 +1310,17 @@
       <c r="I18" s="15">
         <v>187</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="32">
         <f t="shared" si="4"/>
         <v>3.931962690120725</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="21" t="s">
+      <c r="K18" s="33"/>
+    </row>
+    <row r="19" spans="5:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="16">
         <v>285.608</v>
       </c>
@@ -1321,18 +1330,18 @@
       <c r="I19" s="16">
         <v>187</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="36">
         <f t="shared" si="4"/>
         <v>5.7666451920114286</v>
       </c>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="5:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="5:11" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="34" t="s">
+      <c r="K19" s="37"/>
+    </row>
+    <row r="20" spans="5:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="21" spans="5:11" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E21" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="34"/>
+      <c r="F21" s="38"/>
       <c r="G21" s="11" t="s">
         <v>10</v>
       </c>
@@ -1342,16 +1351,16 @@
       <c r="I21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="31" t="s">
+      <c r="J21" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="31"/>
-    </row>
-    <row r="22" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="35" t="s">
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="5:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E22" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="35"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="15">
         <v>183.16900000000001</v>
       </c>
@@ -1361,17 +1370,17 @@
       <c r="I22" s="15">
         <v>0</v>
       </c>
-      <c r="J22" s="32">
+      <c r="J22" s="19">
         <f>(1/(G22))*H22</f>
         <v>0.3111880285419476</v>
       </c>
-      <c r="K22" s="32"/>
-    </row>
-    <row r="23" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="35" t="s">
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="5:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E23" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="35"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="15">
         <v>183.16900000000001</v>
       </c>
@@ -1381,17 +1390,17 @@
       <c r="I23" s="15">
         <v>108</v>
       </c>
-      <c r="J23" s="32">
+      <c r="J23" s="19">
         <f t="shared" ref="J23:J24" si="5">(1/(G23))*H23</f>
         <v>12.873357391261621</v>
       </c>
-      <c r="K23" s="32"/>
-    </row>
-    <row r="24" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="35" t="s">
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="5:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="35"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="15">
         <v>183.16900000000001</v>
       </c>
@@ -1401,17 +1410,59 @@
       <c r="I24" s="15">
         <v>122</v>
       </c>
-      <c r="J24" s="32">
+      <c r="J24" s="19">
         <f t="shared" si="5"/>
         <v>5.7760865648663255</v>
       </c>
-      <c r="K24" s="32"/>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="J27" s="37"/>
+      <c r="K24" s="19"/>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.45">
+      <c r="J27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="E24:F24"/>
@@ -1422,54 +1473,12 @@
     <mergeCell ref="J21:K21"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="J22:K22"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="S7:T7"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>